<commit_message>
update UK news and its related Api document
</commit_message>
<xml_diff>
--- a/development help document /API dictionary.xlsx
+++ b/development help document /API dictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="25600" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="1720" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -175,44 +175,44 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>object</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>it is used to extract keywords from a text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyword_example.py</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>an array of keywords whose item is string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPExtractor(object)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPExtractor('blablablab blabla...')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Currently, when I import it into another python files, it has errors. Perhaps, django is not that wise. I would be working on that. Now, I just paste this code under Ukarticles class to make it work,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jing Qiu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">"in views.py":                                       from .UKNews import UKarticles                                      category=request.GET['category']
-doc = UKarticles.getNewsByCategory(category)               info_dict = UKarticles.getkeywordFromTitle(UKarticles,doc)                                  "in .html file":                                    {{ info_dict.title.0}}                          {{ info_dict.imageUrl.0}} </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>object</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>it is used to extract keywords from a text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>keyword_example.py</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>an array of keywords whose item is string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPExtractor(object)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPExtractor('blablablab blabla...')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Currently, when I import it into another python files, it has errors. Perhaps, django is not that wise. I would be working on that. Now, I just paste this code under Ukarticles class to make it work,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jing Qiu</t>
+info_dict = UKarticles.getNewsByCategory(UKarticles,category)                                "in .html file":                                    {{ info_dict.title.0}}                          {{ info_dict.imageUrl.0}} </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -350,6 +350,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -370,24 +388,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -740,16 +740,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="78" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="51" customHeight="1">
       <c r="A4" s="5" t="s">
@@ -762,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>2</v>
@@ -781,13 +781,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="84" customHeight="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -799,21 +799,21 @@
       <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="142" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="19" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -822,35 +822,35 @@
       <c r="F6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" ht="122" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="22" t="s">
+      <c r="H7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="I7" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>